<commit_message>
Worked some code to pipe to the server models
</commit_message>
<xml_diff>
--- a/Processed Data/Semi_smart_Seal_RBC_TDFS.xlsx
+++ b/Processed Data/Semi_smart_Seal_RBC_TDFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60d52dd049abb4b4/Pictures/Documents/MSc_Seal_SIA/Processed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35CE018E-EE65-42A4-AB17-4BC3EB751769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{35CE018E-EE65-42A4-AB17-4BC3EB751769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3758CFC-F39E-43D5-861C-7E1B39DCB6EA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A86CF68-8C9F-4879-8D4C-0690196077D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>group</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Sandeel</t>
+  </si>
+  <si>
+    <t>Common Dab</t>
+  </si>
+  <si>
+    <t>Plaice</t>
   </si>
 </sst>
 </file>
@@ -426,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E67CFA-EF96-4095-90EF-50BAF015043F}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" customWidth="1"/>
     <col min="3" max="3" width="7.21875" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
@@ -511,7 +517,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1.5</v>
@@ -528,7 +534,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1.5</v>
@@ -545,7 +551,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>1.5</v>
@@ -562,7 +568,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1.5</v>
@@ -579,18 +585,52 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1.5</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="D9">
+        <v>1.7</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1.5</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10">
+        <v>1.7</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>1.5</v>
-      </c>
-      <c r="C9">
-        <v>0.3</v>
-      </c>
-      <c r="D9">
-        <v>1.7</v>
-      </c>
-      <c r="E9">
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11">
+        <v>1.7</v>
+      </c>
+      <c r="E11">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>